<commit_message>
Refactor, eval en, add +100 ru
</commit_message>
<xml_diff>
--- a/sbs/ru_vicuna_question/openai_davinci_003_gusev_7b_ru_alpaca_lora.xlsx
+++ b/sbs/ru_vicuna_question/openai_davinci_003_gusev_7b_ru_alpaca_lora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexkuk/proj/rulm-sbs/sbs/ru_vicuna_question/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B97AD2C-0924-9848-8E2F-31610FAC7E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF7DD1B-F4E1-CB43-A06E-C07D3ED4D85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1742,10 +1742,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1891,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="335" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="335" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1976,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2163,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2282,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2469,7 +2470,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2520,7 +2521,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="272" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2554,7 +2555,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="365" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="288" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2690,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="320" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2843,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2874,10 +2875,10 @@
         <v>199</v>
       </c>
       <c r="E66" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="380" x14ac:dyDescent="0.2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="380" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="320" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2996,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="350" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="335" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="350" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3115,7 +3116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3133,7 +3134,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E81" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>